<commit_message>
Import PG baru, Up Author
</commit_message>
<xml_diff>
--- a/public/template/TemplatePassingGrade.xlsx
+++ b/public/template/TemplatePassingGrade.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Coding\Laravel Project\LangkahEducation\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D997BCBB-F52C-4A04-B67F-AA23145F0165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D72D5D-4E71-418F-B607-AC9642516B3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E59F6822-F562-4972-99D3-7C9765C18367}"/>
   </bookViews>
@@ -31,12 +31,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Prodi</t>
   </si>
   <si>
     <t>Passing Grade</t>
+  </si>
+  <si>
+    <t>Kelompok Passing Grade</t>
   </si>
 </sst>
 </file>
@@ -389,23 +392,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2A0913-E717-47E8-B9B8-6A15D9BF9368}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>